<commit_message>
EV forecast replicated in CyDER project
</commit_message>
<xml_diff>
--- a/cosimulation/static/demo/1_ev_impact/cyder_inputs.xlsx
+++ b/cosimulation/static/demo/1_ev_impact/cyder_inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mygreencar/Desktop/CyDER_vgi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mygreencar/git/CyDER/cosimulation/static/demo/1_ev_impact/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>feeder_name</t>
   </si>
@@ -41,25 +41,34 @@
     <t>timestep</t>
   </si>
   <si>
-    <t>ev_occupancy</t>
-  </si>
-  <si>
     <t>pv_forecast</t>
   </si>
   <si>
-    <t>occupancy_at_node.xlsx</t>
-  </si>
-  <si>
-    <t>vehicle_parameters</t>
-  </si>
-  <si>
-    <t>vehicle_parameters.xlsx</t>
-  </si>
-  <si>
-    <t>load_itineraries</t>
-  </si>
-  <si>
     <t>BU0001</t>
+  </si>
+  <si>
+    <t>ev_forecast</t>
+  </si>
+  <si>
+    <t>transmission_model</t>
+  </si>
+  <si>
+    <t>IEEE_14_bus</t>
+  </si>
+  <si>
+    <t>bus_id</t>
+  </si>
+  <si>
+    <t>add_load</t>
+  </si>
+  <si>
+    <t>add_pv</t>
+  </si>
+  <si>
+    <t>load_forecast</t>
+  </si>
+  <si>
+    <t>static/demo/1_ev_impact/ev_forecast.xlsx</t>
   </si>
 </sst>
 </file>
@@ -384,71 +393,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
+      <c r="D2" s="2">
         <v>42903.25</v>
       </c>
-      <c r="C2" s="2">
+      <c r="E2" s="2">
         <v>42903.875</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>1800</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="b">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="b">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="b">
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>